<commit_message>
Fixed sheet updatation issue
</commit_message>
<xml_diff>
--- a/src/test/resources/DE_HomePage.xlsx
+++ b/src/test/resources/DE_HomePage.xlsx
@@ -114,10 +114,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
+      <selection pane="topLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Updtated data provider code
</commit_message>
<xml_diff>
--- a/src/test/resources/DE_HomePage.xlsx
+++ b/src/test/resources/DE_HomePage.xlsx
@@ -114,10 +114,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
+      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>